<commit_message>
Upload teacher data file
</commit_message>
<xml_diff>
--- a/Admin/TeacherData/LNHS-Teachers.xlsx
+++ b/Admin/TeacherData/LNHS-Teachers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DocMaP\Admin\TeacherData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Corazon\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C625CF-37DC-4C21-B52E-7651FC44E413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD607B6-930D-4461-8076-A6CA3C0626C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{880E497C-C6FD-4B66-B71E-1867D9E57428}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{880E497C-C6FD-4B66-B71E-1867D9E57428}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="152">
   <si>
     <t>Firstname</t>
   </si>
@@ -477,6 +475,21 @@
   </si>
   <si>
     <t>21-77830@g.batstate-u.edu.ph</t>
+  </si>
+  <si>
+    <t>Reynaldo</t>
+  </si>
+  <si>
+    <t>Abiog</t>
+  </si>
+  <si>
+    <t>09918495754</t>
+  </si>
+  <si>
+    <t>abiog.reynaldo10@gmail.com</t>
+  </si>
+  <si>
+    <t>Lumaniag, Lian, Batangas</t>
   </si>
 </sst>
 </file>
@@ -891,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B3BCFB-25E1-4615-A287-0AEB23A92748}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="69" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="69" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1604,8 +1617,34 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="7">
+        <v>23599</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1613,6 +1652,7 @@
     <hyperlink ref="F2" r:id="rId2" xr:uid="{49B4A3DF-CC9C-4BF3-8F1E-6A4E73E43835}"/>
     <hyperlink ref="F23" r:id="rId3" xr:uid="{B97F0638-2170-4C25-AD34-6C30B3FFE580}"/>
     <hyperlink ref="F24" r:id="rId4" xr:uid="{6AC8830F-9D4E-475D-945A-663316A3C81C}"/>
+    <hyperlink ref="F25" r:id="rId5" xr:uid="{69310698-1A3D-44AC-B16F-2E602FF68F11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>